<commit_message>
the last combine 1
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/CombingBillingByJobUSD.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/CombingBillingByJobUSD.xlsx
@@ -647,17 +647,6 @@
     <xf numFmtId="39" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="39" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="39" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="39" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="39" fontId="9" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="39" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="39" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -678,11 +667,63 @@
     <xf numFmtId="39" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="39" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="39" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="39" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="39" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="39" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="39" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -692,9 +733,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="39" fontId="8" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -707,60 +745,22 @@
     <xf numFmtId="39" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="39" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="39" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="39" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="Comma 11" xfId="1"/>
@@ -1107,8 +1107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1138,197 +1138,197 @@
     </row>
     <row r="2" spans="1:23" ht="50.1" customHeight="1">
       <c r="L2" s="36"/>
-      <c r="M2" s="75" t="s">
+      <c r="M2" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="N2" s="75"/>
-      <c r="O2" s="75"/>
-      <c r="P2" s="75"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="46"/>
+      <c r="P2" s="46"/>
       <c r="Q2" s="4"/>
-      <c r="R2" s="46"/>
-      <c r="S2" s="46"/>
-      <c r="T2" s="46"/>
+      <c r="R2" s="41"/>
+      <c r="S2" s="41"/>
+      <c r="T2" s="41"/>
     </row>
     <row r="4" spans="1:23" ht="20.25">
-      <c r="A4" s="76" t="s">
+      <c r="A4" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="76"/>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
-      <c r="F4" s="76"/>
-      <c r="G4" s="76"/>
-      <c r="H4" s="76"/>
-      <c r="I4" s="76"/>
-      <c r="J4" s="76"/>
-      <c r="K4" s="76"/>
-      <c r="L4" s="76"/>
-      <c r="M4" s="76"/>
-      <c r="N4" s="76"/>
-      <c r="O4" s="76"/>
-      <c r="P4" s="76"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="47"/>
+      <c r="M4" s="47"/>
+      <c r="N4" s="47"/>
+      <c r="O4" s="47"/>
+      <c r="P4" s="47"/>
       <c r="Q4" s="5"/>
-      <c r="R4" s="47"/>
-      <c r="S4" s="47"/>
-      <c r="T4" s="47"/>
+      <c r="R4" s="42"/>
+      <c r="S4" s="42"/>
+      <c r="T4" s="42"/>
     </row>
     <row r="5" spans="1:23" ht="18.75">
-      <c r="A5" s="77" t="s">
+      <c r="A5" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="78"/>
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="78"/>
-      <c r="H5" s="78"/>
-      <c r="I5" s="78"/>
-      <c r="J5" s="78"/>
-      <c r="K5" s="78"/>
-      <c r="L5" s="78"/>
-      <c r="M5" s="78"/>
-      <c r="N5" s="78"/>
-      <c r="O5" s="78"/>
-      <c r="P5" s="78"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="49"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="49"/>
+      <c r="N5" s="49"/>
+      <c r="O5" s="49"/>
+      <c r="P5" s="49"/>
       <c r="Q5" s="6"/>
-      <c r="R5" s="48"/>
-      <c r="S5" s="48"/>
-      <c r="T5" s="48"/>
+      <c r="R5" s="43"/>
+      <c r="S5" s="43"/>
+      <c r="T5" s="43"/>
     </row>
     <row r="6" spans="1:23" ht="19.5">
-      <c r="A6" s="79" t="s">
+      <c r="A6" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="79"/>
-      <c r="C6" s="79"/>
-      <c r="D6" s="79"/>
-      <c r="E6" s="79"/>
-      <c r="F6" s="79"/>
-      <c r="G6" s="79"/>
-      <c r="H6" s="79"/>
-      <c r="I6" s="79"/>
-      <c r="J6" s="79"/>
-      <c r="K6" s="79"/>
-      <c r="L6" s="79"/>
-      <c r="M6" s="79"/>
-      <c r="N6" s="79"/>
-      <c r="O6" s="79"/>
-      <c r="P6" s="79"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="50"/>
+      <c r="J6" s="50"/>
+      <c r="K6" s="50"/>
+      <c r="L6" s="50"/>
+      <c r="M6" s="50"/>
+      <c r="N6" s="50"/>
+      <c r="O6" s="50"/>
+      <c r="P6" s="50"/>
       <c r="Q6" s="7"/>
-      <c r="R6" s="49"/>
-      <c r="S6" s="49"/>
-      <c r="T6" s="49"/>
+      <c r="R6" s="44"/>
+      <c r="S6" s="44"/>
+      <c r="T6" s="44"/>
     </row>
     <row r="7" spans="1:23" ht="19.5">
-      <c r="A7" s="79" t="s">
+      <c r="A7" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="79"/>
-      <c r="C7" s="79"/>
-      <c r="D7" s="79"/>
-      <c r="E7" s="79"/>
-      <c r="F7" s="79"/>
-      <c r="G7" s="79"/>
-      <c r="H7" s="79"/>
-      <c r="I7" s="79"/>
-      <c r="J7" s="79"/>
-      <c r="K7" s="79"/>
-      <c r="L7" s="79"/>
-      <c r="M7" s="79"/>
-      <c r="N7" s="79"/>
-      <c r="O7" s="79"/>
-      <c r="P7" s="79"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="50"/>
+      <c r="N7" s="50"/>
+      <c r="O7" s="50"/>
+      <c r="P7" s="50"/>
       <c r="Q7" s="7"/>
-      <c r="R7" s="49"/>
-      <c r="S7" s="49"/>
-      <c r="T7" s="49"/>
+      <c r="R7" s="44"/>
+      <c r="S7" s="44"/>
+      <c r="T7" s="44"/>
     </row>
     <row r="8" spans="1:23" ht="13.5" thickBot="1">
-      <c r="A8" s="54" t="s">
+      <c r="A8" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="54"/>
-      <c r="C8" s="54"/>
-      <c r="D8" s="54"/>
-      <c r="E8" s="54"/>
-      <c r="F8" s="54"/>
-      <c r="G8" s="54"/>
-      <c r="H8" s="54"/>
-      <c r="I8" s="54"/>
-      <c r="J8" s="54"/>
-      <c r="K8" s="54"/>
-      <c r="L8" s="54"/>
-      <c r="M8" s="54"/>
-      <c r="N8" s="54"/>
-      <c r="O8" s="54"/>
-      <c r="P8" s="54"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="65"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="65"/>
+      <c r="G8" s="65"/>
+      <c r="H8" s="65"/>
+      <c r="I8" s="65"/>
+      <c r="J8" s="65"/>
+      <c r="K8" s="65"/>
+      <c r="L8" s="65"/>
+      <c r="M8" s="65"/>
+      <c r="N8" s="65"/>
+      <c r="O8" s="65"/>
+      <c r="P8" s="65"/>
       <c r="Q8" s="8"/>
-      <c r="R8" s="50"/>
-      <c r="S8" s="50"/>
-      <c r="T8" s="50"/>
+      <c r="R8" s="45"/>
+      <c r="S8" s="45"/>
+      <c r="T8" s="45"/>
     </row>
     <row r="9" spans="1:23" s="1" customFormat="1" ht="36.75" customHeight="1">
-      <c r="A9" s="72" t="s">
+      <c r="A9" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="57" t="s">
+      <c r="B9" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="57" t="s">
+      <c r="C9" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="57" t="s">
+      <c r="D9" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="57" t="s">
+      <c r="E9" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="57" t="s">
+      <c r="F9" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="55" t="s">
+      <c r="G9" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="56"/>
-      <c r="I9" s="57"/>
-      <c r="J9" s="58" t="s">
+      <c r="H9" s="67"/>
+      <c r="I9" s="59"/>
+      <c r="J9" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="59"/>
-      <c r="L9" s="60"/>
-      <c r="M9" s="58" t="s">
+      <c r="K9" s="69"/>
+      <c r="L9" s="70"/>
+      <c r="M9" s="68" t="s">
         <v>11</v>
       </c>
-      <c r="N9" s="59"/>
-      <c r="O9" s="60"/>
-      <c r="P9" s="61" t="s">
+      <c r="N9" s="69"/>
+      <c r="O9" s="70"/>
+      <c r="P9" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="Q9" s="67" t="s">
+      <c r="Q9" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="R9" s="68"/>
-      <c r="S9" s="68"/>
-      <c r="T9" s="69"/>
-      <c r="U9" s="74" t="s">
+      <c r="R9" s="55"/>
+      <c r="S9" s="55"/>
+      <c r="T9" s="56"/>
+      <c r="U9" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="V9" s="64" t="s">
+      <c r="V9" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="W9" s="66" t="s">
+      <c r="W9" s="53" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:23" s="1" customFormat="1" ht="36.75" customHeight="1">
-      <c r="A10" s="73"/>
-      <c r="B10" s="63"/>
-      <c r="C10" s="63"/>
-      <c r="D10" s="63"/>
-      <c r="E10" s="63"/>
-      <c r="F10" s="63"/>
+      <c r="A10" s="62"/>
+      <c r="B10" s="60"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="60"/>
+      <c r="F10" s="60"/>
       <c r="G10" s="2" t="s">
         <v>17</v>
       </c>
@@ -1356,7 +1356,7 @@
       <c r="O10" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="P10" s="62"/>
+      <c r="P10" s="64"/>
       <c r="Q10" s="12" t="s">
         <v>22</v>
       </c>
@@ -1369,9 +1369,9 @@
       <c r="T10" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="U10" s="62"/>
-      <c r="V10" s="65"/>
-      <c r="W10" s="66"/>
+      <c r="U10" s="64"/>
+      <c r="V10" s="52"/>
+      <c r="W10" s="53"/>
     </row>
     <row r="11" spans="1:23" s="3" customFormat="1" ht="16.5" customHeight="1">
       <c r="A11" s="21" t="s">
@@ -1401,40 +1401,40 @@
       <c r="I11" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="J11" s="38" t="s">
+      <c r="J11" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="K11" s="38" t="s">
+      <c r="K11" s="72" t="s">
         <v>35</v>
       </c>
-      <c r="L11" s="38" t="s">
+      <c r="L11" s="72" t="s">
         <v>46</v>
       </c>
-      <c r="M11" s="38" t="s">
+      <c r="M11" s="72" t="s">
         <v>36</v>
       </c>
-      <c r="N11" s="38" t="s">
+      <c r="N11" s="72" t="s">
         <v>37</v>
       </c>
-      <c r="O11" s="38" t="s">
+      <c r="O11" s="72" t="s">
         <v>47</v>
       </c>
-      <c r="P11" s="39" t="s">
+      <c r="P11" s="73" t="s">
         <v>48</v>
       </c>
       <c r="Q11" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="R11" s="51" t="s">
+      <c r="R11" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="S11" s="51" t="s">
+      <c r="S11" s="77" t="s">
         <v>39</v>
       </c>
-      <c r="T11" s="38" t="s">
+      <c r="T11" s="72" t="s">
         <v>49</v>
       </c>
-      <c r="U11" s="39" t="s">
+      <c r="U11" s="73" t="s">
         <v>50</v>
       </c>
       <c r="V11" s="26" t="s">
@@ -1454,75 +1454,75 @@
       <c r="G12" s="30"/>
       <c r="H12" s="18"/>
       <c r="I12" s="20"/>
-      <c r="J12" s="40"/>
-      <c r="K12" s="40"/>
-      <c r="L12" s="40"/>
-      <c r="M12" s="40"/>
-      <c r="N12" s="40"/>
-      <c r="O12" s="40"/>
-      <c r="P12" s="41"/>
+      <c r="J12" s="74"/>
+      <c r="K12" s="74"/>
+      <c r="L12" s="74"/>
+      <c r="M12" s="74"/>
+      <c r="N12" s="74"/>
+      <c r="O12" s="74"/>
+      <c r="P12" s="75"/>
       <c r="Q12" s="31"/>
-      <c r="R12" s="52"/>
-      <c r="S12" s="52"/>
-      <c r="T12" s="53"/>
-      <c r="U12" s="41"/>
+      <c r="R12" s="78"/>
+      <c r="S12" s="78"/>
+      <c r="T12" s="79"/>
+      <c r="U12" s="75"/>
       <c r="V12" s="15"/>
       <c r="W12" s="14"/>
     </row>
     <row r="13" spans="1:23" s="1" customFormat="1" ht="36" customHeight="1" thickBot="1">
-      <c r="A13" s="70" t="s">
+      <c r="A13" s="57" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="71"/>
-      <c r="C13" s="71"/>
-      <c r="D13" s="71"/>
-      <c r="E13" s="71"/>
-      <c r="F13" s="71"/>
-      <c r="G13" s="71"/>
-      <c r="H13" s="71"/>
-      <c r="I13" s="71"/>
-      <c r="J13" s="42">
-        <f t="shared" ref="J13:P13" si="0">SUM(J11:J12)</f>
+      <c r="B13" s="58"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="58"/>
+      <c r="E13" s="58"/>
+      <c r="F13" s="58"/>
+      <c r="G13" s="58"/>
+      <c r="H13" s="58"/>
+      <c r="I13" s="58"/>
+      <c r="J13" s="76">
+        <f t="shared" ref="J13:N13" si="0">SUM(J11:J12)</f>
         <v>0</v>
       </c>
-      <c r="K13" s="42">
+      <c r="K13" s="76">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L13" s="42">
+      <c r="L13" s="76">
         <f>SUM(L11:L12)</f>
         <v>0</v>
       </c>
-      <c r="M13" s="42">
+      <c r="M13" s="76">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N13" s="42">
+      <c r="N13" s="76">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O13" s="42">
+      <c r="O13" s="76">
         <f>SUM(O11:O12)</f>
         <v>0</v>
       </c>
-      <c r="P13" s="42">
+      <c r="P13" s="76">
         <f>SUM(P11:P12)</f>
         <v>0</v>
       </c>
       <c r="Q13" s="32"/>
-      <c r="R13" s="42">
+      <c r="R13" s="76">
         <f>SUM(R11:R12)</f>
         <v>0</v>
       </c>
-      <c r="S13" s="42">
+      <c r="S13" s="76">
         <f>SUM(S11:S12)</f>
         <v>0</v>
       </c>
-      <c r="T13" s="42">
+      <c r="T13" s="76">
         <f>SUM(T11:T12)</f>
         <v>0</v>
       </c>
-      <c r="U13" s="42">
+      <c r="U13" s="76">
         <f>SUM(U11:U12)</f>
         <v>0</v>
       </c>
@@ -1530,49 +1530,51 @@
       <c r="W13" s="13"/>
     </row>
     <row r="14" spans="1:23" ht="15.75">
-      <c r="N14" s="43"/>
-      <c r="O14" s="43"/>
-      <c r="P14" s="43"/>
+      <c r="N14" s="38"/>
+      <c r="O14" s="38"/>
+      <c r="P14" s="38"/>
       <c r="Q14" s="9"/>
     </row>
     <row r="15" spans="1:23" ht="15.75">
-      <c r="N15" s="44"/>
-      <c r="O15" s="44"/>
-      <c r="P15" s="44"/>
+      <c r="N15" s="39"/>
+      <c r="O15" s="39"/>
+      <c r="P15" s="39"/>
       <c r="Q15" s="10"/>
     </row>
     <row r="16" spans="1:23" ht="15.75">
-      <c r="N16" s="44"/>
-      <c r="O16" s="44"/>
-      <c r="P16" s="44"/>
+      <c r="N16" s="39"/>
+      <c r="O16" s="39"/>
+      <c r="P16" s="39"/>
       <c r="Q16" s="10"/>
     </row>
     <row r="17" spans="14:17" ht="15.75">
-      <c r="N17" s="44"/>
-      <c r="O17" s="44"/>
-      <c r="P17" s="44"/>
+      <c r="N17" s="39"/>
+      <c r="O17" s="39"/>
+      <c r="P17" s="39"/>
       <c r="Q17" s="10"/>
     </row>
     <row r="18" spans="14:17" ht="15.75">
-      <c r="N18" s="45"/>
-      <c r="O18" s="45"/>
-      <c r="P18" s="45"/>
+      <c r="N18" s="40"/>
+      <c r="O18" s="40"/>
+      <c r="P18" s="40"/>
       <c r="Q18" s="11"/>
     </row>
     <row r="19" spans="14:17" ht="15.75">
-      <c r="N19" s="45"/>
-      <c r="O19" s="45"/>
-      <c r="P19" s="45"/>
+      <c r="N19" s="40"/>
+      <c r="O19" s="40"/>
+      <c r="P19" s="40"/>
       <c r="Q19" s="11"/>
     </row>
   </sheetData>
   <autoFilter ref="A9:W10"/>
   <mergeCells count="21">
-    <mergeCell ref="M2:P2"/>
-    <mergeCell ref="A4:P4"/>
-    <mergeCell ref="A5:P5"/>
-    <mergeCell ref="A6:P6"/>
-    <mergeCell ref="A7:P7"/>
+    <mergeCell ref="A8:P8"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
     <mergeCell ref="V9:V10"/>
     <mergeCell ref="W9:W10"/>
     <mergeCell ref="Q9:T9"/>
@@ -1582,13 +1584,11 @@
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="U9:U10"/>
-    <mergeCell ref="A8:P8"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="M9:O9"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="A4:P4"/>
+    <mergeCell ref="A5:P5"/>
+    <mergeCell ref="A6:P6"/>
+    <mergeCell ref="A7:P7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
reformat form combine billing by shipment
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/CombingBillingByJobUSD.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/CombingBillingByJobUSD.xlsx
@@ -566,7 +566,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -607,17 +607,11 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -629,9 +623,6 @@
     <xf numFmtId="1" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="37" fontId="9" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="37" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -667,84 +658,6 @@
     <xf numFmtId="39" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="39" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="39" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="39" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="39" fontId="8" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="39" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="39" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="39" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -761,6 +674,90 @@
     </xf>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="39" fontId="8" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="39" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="39" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="39" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="39" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="39" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="39" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="Comma 11" xfId="1"/>
@@ -1108,7 +1105,7 @@
   <dimension ref="A1:W19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:I13"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1121,209 +1118,209 @@
     <col min="6" max="6" width="29" customWidth="1"/>
     <col min="7" max="8" width="14" customWidth="1"/>
     <col min="9" max="9" width="16.5703125" customWidth="1"/>
-    <col min="10" max="16" width="20" style="34" customWidth="1"/>
+    <col min="10" max="16" width="20" style="31" customWidth="1"/>
     <col min="17" max="17" width="35.7109375" customWidth="1"/>
-    <col min="18" max="18" width="12.42578125" style="34" customWidth="1"/>
-    <col min="19" max="19" width="13" style="34" customWidth="1"/>
-    <col min="20" max="20" width="20" style="34" customWidth="1"/>
-    <col min="21" max="21" width="22" style="34" customWidth="1"/>
+    <col min="18" max="18" width="12.42578125" style="31" customWidth="1"/>
+    <col min="19" max="19" width="13" style="31" customWidth="1"/>
+    <col min="20" max="20" width="20" style="31" customWidth="1"/>
+    <col min="21" max="21" width="22" style="31" customWidth="1"/>
     <col min="22" max="22" width="15.85546875" customWidth="1"/>
     <col min="23" max="23" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="20.25">
-      <c r="M1" s="35" t="s">
+      <c r="M1" s="32" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="50.1" customHeight="1">
-      <c r="L2" s="36"/>
-      <c r="M2" s="46" t="s">
+      <c r="L2" s="33"/>
+      <c r="M2" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
+      <c r="N2" s="72"/>
+      <c r="O2" s="72"/>
+      <c r="P2" s="72"/>
       <c r="Q2" s="4"/>
-      <c r="R2" s="41"/>
-      <c r="S2" s="41"/>
-      <c r="T2" s="41"/>
+      <c r="R2" s="38"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="38"/>
     </row>
     <row r="4" spans="1:23" ht="20.25">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="47"/>
-      <c r="M4" s="47"/>
-      <c r="N4" s="47"/>
-      <c r="O4" s="47"/>
-      <c r="P4" s="47"/>
+      <c r="B4" s="73"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="73"/>
+      <c r="J4" s="73"/>
+      <c r="K4" s="73"/>
+      <c r="L4" s="73"/>
+      <c r="M4" s="73"/>
+      <c r="N4" s="73"/>
+      <c r="O4" s="73"/>
+      <c r="P4" s="73"/>
       <c r="Q4" s="5"/>
-      <c r="R4" s="42"/>
-      <c r="S4" s="42"/>
-      <c r="T4" s="42"/>
+      <c r="R4" s="39"/>
+      <c r="S4" s="39"/>
+      <c r="T4" s="39"/>
     </row>
     <row r="5" spans="1:23" ht="18.75">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="74" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="49"/>
-      <c r="L5" s="49"/>
-      <c r="M5" s="49"/>
-      <c r="N5" s="49"/>
-      <c r="O5" s="49"/>
-      <c r="P5" s="49"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="75"/>
+      <c r="I5" s="75"/>
+      <c r="J5" s="75"/>
+      <c r="K5" s="75"/>
+      <c r="L5" s="75"/>
+      <c r="M5" s="75"/>
+      <c r="N5" s="75"/>
+      <c r="O5" s="75"/>
+      <c r="P5" s="75"/>
       <c r="Q5" s="6"/>
-      <c r="R5" s="43"/>
-      <c r="S5" s="43"/>
-      <c r="T5" s="43"/>
+      <c r="R5" s="40"/>
+      <c r="S5" s="40"/>
+      <c r="T5" s="40"/>
     </row>
     <row r="6" spans="1:23" ht="19.5">
-      <c r="A6" s="50" t="s">
+      <c r="A6" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="50"/>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="50"/>
-      <c r="H6" s="50"/>
-      <c r="I6" s="50"/>
-      <c r="J6" s="50"/>
-      <c r="K6" s="50"/>
-      <c r="L6" s="50"/>
-      <c r="M6" s="50"/>
-      <c r="N6" s="50"/>
-      <c r="O6" s="50"/>
-      <c r="P6" s="50"/>
+      <c r="B6" s="76"/>
+      <c r="C6" s="76"/>
+      <c r="D6" s="76"/>
+      <c r="E6" s="76"/>
+      <c r="F6" s="76"/>
+      <c r="G6" s="76"/>
+      <c r="H6" s="76"/>
+      <c r="I6" s="76"/>
+      <c r="J6" s="76"/>
+      <c r="K6" s="76"/>
+      <c r="L6" s="76"/>
+      <c r="M6" s="76"/>
+      <c r="N6" s="76"/>
+      <c r="O6" s="76"/>
+      <c r="P6" s="76"/>
       <c r="Q6" s="7"/>
-      <c r="R6" s="44"/>
-      <c r="S6" s="44"/>
-      <c r="T6" s="44"/>
+      <c r="R6" s="41"/>
+      <c r="S6" s="41"/>
+      <c r="T6" s="41"/>
     </row>
     <row r="7" spans="1:23" ht="19.5">
-      <c r="A7" s="50" t="s">
+      <c r="A7" s="76" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="50"/>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="50"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="50"/>
-      <c r="J7" s="50"/>
-      <c r="K7" s="50"/>
-      <c r="L7" s="50"/>
-      <c r="M7" s="50"/>
-      <c r="N7" s="50"/>
-      <c r="O7" s="50"/>
-      <c r="P7" s="50"/>
+      <c r="B7" s="76"/>
+      <c r="C7" s="76"/>
+      <c r="D7" s="76"/>
+      <c r="E7" s="76"/>
+      <c r="F7" s="76"/>
+      <c r="G7" s="76"/>
+      <c r="H7" s="76"/>
+      <c r="I7" s="76"/>
+      <c r="J7" s="76"/>
+      <c r="K7" s="76"/>
+      <c r="L7" s="76"/>
+      <c r="M7" s="76"/>
+      <c r="N7" s="76"/>
+      <c r="O7" s="76"/>
+      <c r="P7" s="76"/>
       <c r="Q7" s="7"/>
-      <c r="R7" s="44"/>
-      <c r="S7" s="44"/>
-      <c r="T7" s="44"/>
+      <c r="R7" s="41"/>
+      <c r="S7" s="41"/>
+      <c r="T7" s="41"/>
     </row>
     <row r="8" spans="1:23" ht="13.5" thickBot="1">
-      <c r="A8" s="65" t="s">
+      <c r="A8" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="65"/>
-      <c r="C8" s="65"/>
-      <c r="D8" s="65"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="65"/>
-      <c r="G8" s="65"/>
-      <c r="H8" s="65"/>
-      <c r="I8" s="65"/>
-      <c r="J8" s="65"/>
-      <c r="K8" s="65"/>
-      <c r="L8" s="65"/>
-      <c r="M8" s="65"/>
-      <c r="N8" s="65"/>
-      <c r="O8" s="65"/>
-      <c r="P8" s="65"/>
+      <c r="B8" s="51"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="51"/>
+      <c r="F8" s="51"/>
+      <c r="G8" s="51"/>
+      <c r="H8" s="51"/>
+      <c r="I8" s="51"/>
+      <c r="J8" s="51"/>
+      <c r="K8" s="51"/>
+      <c r="L8" s="51"/>
+      <c r="M8" s="51"/>
+      <c r="N8" s="51"/>
+      <c r="O8" s="51"/>
+      <c r="P8" s="51"/>
       <c r="Q8" s="8"/>
-      <c r="R8" s="45"/>
-      <c r="S8" s="45"/>
-      <c r="T8" s="45"/>
+      <c r="R8" s="42"/>
+      <c r="S8" s="42"/>
+      <c r="T8" s="42"/>
     </row>
     <row r="9" spans="1:23" s="1" customFormat="1" ht="36.75" customHeight="1">
-      <c r="A9" s="61" t="s">
+      <c r="A9" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="59" t="s">
+      <c r="B9" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="59" t="s">
+      <c r="C9" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="59" t="s">
+      <c r="D9" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="59" t="s">
+      <c r="E9" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="59" t="s">
+      <c r="F9" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="66" t="s">
+      <c r="G9" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="67"/>
-      <c r="I9" s="59"/>
-      <c r="J9" s="68" t="s">
+      <c r="H9" s="53"/>
+      <c r="I9" s="54"/>
+      <c r="J9" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="69"/>
-      <c r="L9" s="70"/>
-      <c r="M9" s="68" t="s">
+      <c r="K9" s="56"/>
+      <c r="L9" s="57"/>
+      <c r="M9" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="N9" s="69"/>
-      <c r="O9" s="70"/>
-      <c r="P9" s="71" t="s">
+      <c r="N9" s="56"/>
+      <c r="O9" s="57"/>
+      <c r="P9" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="Q9" s="54" t="s">
+      <c r="Q9" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="R9" s="55"/>
-      <c r="S9" s="55"/>
-      <c r="T9" s="56"/>
-      <c r="U9" s="63" t="s">
+      <c r="R9" s="65"/>
+      <c r="S9" s="65"/>
+      <c r="T9" s="66"/>
+      <c r="U9" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="V9" s="51" t="s">
+      <c r="V9" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="W9" s="53" t="s">
+      <c r="W9" s="63" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:23" s="1" customFormat="1" ht="36.75" customHeight="1">
-      <c r="A10" s="62"/>
+      <c r="A10" s="70"/>
       <c r="B10" s="60"/>
       <c r="C10" s="60"/>
       <c r="D10" s="60"/>
@@ -1338,109 +1335,109 @@
       <c r="I10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="37" t="s">
+      <c r="J10" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="K10" s="37" t="s">
+      <c r="K10" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="L10" s="37" t="s">
+      <c r="L10" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="M10" s="37" t="s">
+      <c r="M10" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="N10" s="37" t="s">
+      <c r="N10" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="O10" s="37" t="s">
+      <c r="O10" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="P10" s="64"/>
+      <c r="P10" s="59"/>
       <c r="Q10" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="R10" s="37" t="s">
+      <c r="R10" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="S10" s="37" t="s">
+      <c r="S10" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="T10" s="37" t="s">
+      <c r="T10" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="U10" s="64"/>
-      <c r="V10" s="52"/>
-      <c r="W10" s="53"/>
+      <c r="U10" s="59"/>
+      <c r="V10" s="62"/>
+      <c r="W10" s="63"/>
     </row>
     <row r="11" spans="1:23" s="3" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="28" t="s">
+      <c r="D11" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="25" t="s">
+      <c r="E11" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="23" t="s">
+      <c r="F11" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="G11" s="28" t="s">
+      <c r="G11" s="77" t="s">
         <v>42</v>
       </c>
-      <c r="H11" s="23" t="s">
+      <c r="H11" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="I11" s="24" t="s">
+      <c r="I11" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="J11" s="72" t="s">
+      <c r="J11" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="K11" s="72" t="s">
+      <c r="K11" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="L11" s="72" t="s">
+      <c r="L11" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="M11" s="72" t="s">
+      <c r="M11" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="N11" s="72" t="s">
+      <c r="N11" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="O11" s="72" t="s">
+      <c r="O11" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="P11" s="73" t="s">
+      <c r="P11" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="Q11" s="33" t="s">
+      <c r="Q11" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="R11" s="77" t="s">
+      <c r="R11" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="S11" s="77" t="s">
+      <c r="S11" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="T11" s="72" t="s">
+      <c r="T11" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="U11" s="73" t="s">
+      <c r="U11" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="V11" s="26" t="s">
+      <c r="V11" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="W11" s="27" t="s">
+      <c r="W11" s="25" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1448,81 +1445,81 @@
       <c r="A12" s="16"/>
       <c r="B12" s="17"/>
       <c r="C12" s="18"/>
-      <c r="D12" s="29"/>
+      <c r="D12" s="27"/>
       <c r="E12" s="19"/>
       <c r="F12" s="18"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="74"/>
-      <c r="K12" s="74"/>
-      <c r="L12" s="74"/>
-      <c r="M12" s="74"/>
-      <c r="N12" s="74"/>
-      <c r="O12" s="74"/>
-      <c r="P12" s="75"/>
-      <c r="Q12" s="31"/>
-      <c r="R12" s="78"/>
-      <c r="S12" s="78"/>
-      <c r="T12" s="79"/>
-      <c r="U12" s="75"/>
+      <c r="G12" s="78"/>
+      <c r="H12" s="78"/>
+      <c r="I12" s="78"/>
+      <c r="J12" s="45"/>
+      <c r="K12" s="45"/>
+      <c r="L12" s="45"/>
+      <c r="M12" s="45"/>
+      <c r="N12" s="45"/>
+      <c r="O12" s="45"/>
+      <c r="P12" s="46"/>
+      <c r="Q12" s="28"/>
+      <c r="R12" s="49"/>
+      <c r="S12" s="49"/>
+      <c r="T12" s="50"/>
+      <c r="U12" s="46"/>
       <c r="V12" s="15"/>
       <c r="W12" s="14"/>
     </row>
     <row r="13" spans="1:23" s="1" customFormat="1" ht="36" customHeight="1" thickBot="1">
-      <c r="A13" s="57" t="s">
+      <c r="A13" s="67" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="58"/>
-      <c r="C13" s="58"/>
-      <c r="D13" s="58"/>
-      <c r="E13" s="58"/>
-      <c r="F13" s="58"/>
-      <c r="G13" s="58"/>
-      <c r="H13" s="58"/>
-      <c r="I13" s="58"/>
-      <c r="J13" s="76">
+      <c r="B13" s="68"/>
+      <c r="C13" s="68"/>
+      <c r="D13" s="68"/>
+      <c r="E13" s="68"/>
+      <c r="F13" s="68"/>
+      <c r="G13" s="68"/>
+      <c r="H13" s="68"/>
+      <c r="I13" s="68"/>
+      <c r="J13" s="47">
         <f t="shared" ref="J13:N13" si="0">SUM(J11:J12)</f>
         <v>0</v>
       </c>
-      <c r="K13" s="76">
+      <c r="K13" s="47">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L13" s="76">
+      <c r="L13" s="47">
         <f>SUM(L11:L12)</f>
         <v>0</v>
       </c>
-      <c r="M13" s="76">
+      <c r="M13" s="47">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N13" s="76">
+      <c r="N13" s="47">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O13" s="76">
+      <c r="O13" s="47">
         <f>SUM(O11:O12)</f>
         <v>0</v>
       </c>
-      <c r="P13" s="76">
+      <c r="P13" s="47">
         <f>SUM(P11:P12)</f>
         <v>0</v>
       </c>
-      <c r="Q13" s="32"/>
-      <c r="R13" s="76">
+      <c r="Q13" s="29"/>
+      <c r="R13" s="47">
         <f>SUM(R11:R12)</f>
         <v>0</v>
       </c>
-      <c r="S13" s="76">
+      <c r="S13" s="47">
         <f>SUM(S11:S12)</f>
         <v>0</v>
       </c>
-      <c r="T13" s="76">
+      <c r="T13" s="47">
         <f>SUM(T11:T12)</f>
         <v>0</v>
       </c>
-      <c r="U13" s="76">
+      <c r="U13" s="47">
         <f>SUM(U11:U12)</f>
         <v>0</v>
       </c>
@@ -1530,51 +1527,49 @@
       <c r="W13" s="13"/>
     </row>
     <row r="14" spans="1:23" ht="15.75">
-      <c r="N14" s="38"/>
-      <c r="O14" s="38"/>
-      <c r="P14" s="38"/>
+      <c r="N14" s="35"/>
+      <c r="O14" s="35"/>
+      <c r="P14" s="35"/>
       <c r="Q14" s="9"/>
     </row>
     <row r="15" spans="1:23" ht="15.75">
-      <c r="N15" s="39"/>
-      <c r="O15" s="39"/>
-      <c r="P15" s="39"/>
+      <c r="N15" s="36"/>
+      <c r="O15" s="36"/>
+      <c r="P15" s="36"/>
       <c r="Q15" s="10"/>
     </row>
     <row r="16" spans="1:23" ht="15.75">
-      <c r="N16" s="39"/>
-      <c r="O16" s="39"/>
-      <c r="P16" s="39"/>
+      <c r="N16" s="36"/>
+      <c r="O16" s="36"/>
+      <c r="P16" s="36"/>
       <c r="Q16" s="10"/>
     </row>
     <row r="17" spans="14:17" ht="15.75">
-      <c r="N17" s="39"/>
-      <c r="O17" s="39"/>
-      <c r="P17" s="39"/>
+      <c r="N17" s="36"/>
+      <c r="O17" s="36"/>
+      <c r="P17" s="36"/>
       <c r="Q17" s="10"/>
     </row>
     <row r="18" spans="14:17" ht="15.75">
-      <c r="N18" s="40"/>
-      <c r="O18" s="40"/>
-      <c r="P18" s="40"/>
+      <c r="N18" s="37"/>
+      <c r="O18" s="37"/>
+      <c r="P18" s="37"/>
       <c r="Q18" s="11"/>
     </row>
     <row r="19" spans="14:17" ht="15.75">
-      <c r="N19" s="40"/>
-      <c r="O19" s="40"/>
-      <c r="P19" s="40"/>
+      <c r="N19" s="37"/>
+      <c r="O19" s="37"/>
+      <c r="P19" s="37"/>
       <c r="Q19" s="11"/>
     </row>
   </sheetData>
   <autoFilter ref="A9:W10"/>
   <mergeCells count="21">
-    <mergeCell ref="A8:P8"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="M9:O9"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="A4:P4"/>
+    <mergeCell ref="A5:P5"/>
+    <mergeCell ref="A6:P6"/>
+    <mergeCell ref="A7:P7"/>
     <mergeCell ref="V9:V10"/>
     <mergeCell ref="W9:W10"/>
     <mergeCell ref="Q9:T9"/>
@@ -1584,11 +1579,13 @@
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="U9:U10"/>
-    <mergeCell ref="M2:P2"/>
-    <mergeCell ref="A4:P4"/>
-    <mergeCell ref="A5:P5"/>
-    <mergeCell ref="A6:P6"/>
-    <mergeCell ref="A7:P7"/>
+    <mergeCell ref="A8:P8"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add Service Date for combine exprot template
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/CombingBillingByJobUSD.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/CombingBillingByJobUSD.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
   <si>
     <t>INDO TRANS LOGISTICS CORPORATION</t>
   </si>
@@ -190,6 +190,12 @@
   </si>
   <si>
     <t>{PTTotal}</t>
+  </si>
+  <si>
+    <t>{ServiceDate}</t>
+  </si>
+  <si>
+    <t>Service Date</t>
   </si>
 </sst>
 </file>
@@ -566,7 +572,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -667,84 +673,6 @@
     <xf numFmtId="39" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="39" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="39" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="39" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="39" fontId="8" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="39" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="39" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="39" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -761,6 +689,87 @@
     </xf>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="39" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="39" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="39" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="39" fontId="8" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="39" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="39" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="39" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="Comma 11" xfId="1"/>
@@ -1105,10 +1114,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W19"/>
+  <dimension ref="A1:X19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:I13"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="X18" sqref="X18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1129,206 +1138,210 @@
     <col min="21" max="21" width="22" style="34" customWidth="1"/>
     <col min="22" max="22" width="15.85546875" customWidth="1"/>
     <col min="23" max="23" width="14.42578125" customWidth="1"/>
+    <col min="24" max="24" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="20.25">
+    <row r="1" spans="1:24" ht="20.25">
       <c r="M1" s="35" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="50.1" customHeight="1">
+    <row r="2" spans="1:24" ht="50.1" customHeight="1">
       <c r="L2" s="36"/>
-      <c r="M2" s="46" t="s">
+      <c r="M2" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="55"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="41"/>
       <c r="S2" s="41"/>
       <c r="T2" s="41"/>
     </row>
-    <row r="4" spans="1:23" ht="20.25">
-      <c r="A4" s="47" t="s">
+    <row r="4" spans="1:24" ht="20.25">
+      <c r="A4" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="47"/>
-      <c r="M4" s="47"/>
-      <c r="N4" s="47"/>
-      <c r="O4" s="47"/>
-      <c r="P4" s="47"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="56"/>
+      <c r="J4" s="56"/>
+      <c r="K4" s="56"/>
+      <c r="L4" s="56"/>
+      <c r="M4" s="56"/>
+      <c r="N4" s="56"/>
+      <c r="O4" s="56"/>
+      <c r="P4" s="56"/>
       <c r="Q4" s="5"/>
       <c r="R4" s="42"/>
       <c r="S4" s="42"/>
       <c r="T4" s="42"/>
     </row>
-    <row r="5" spans="1:23" ht="18.75">
-      <c r="A5" s="48" t="s">
+    <row r="5" spans="1:24" ht="18.75">
+      <c r="A5" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="49"/>
-      <c r="L5" s="49"/>
-      <c r="M5" s="49"/>
-      <c r="N5" s="49"/>
-      <c r="O5" s="49"/>
-      <c r="P5" s="49"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="58"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="58"/>
+      <c r="K5" s="58"/>
+      <c r="L5" s="58"/>
+      <c r="M5" s="58"/>
+      <c r="N5" s="58"/>
+      <c r="O5" s="58"/>
+      <c r="P5" s="58"/>
       <c r="Q5" s="6"/>
       <c r="R5" s="43"/>
       <c r="S5" s="43"/>
       <c r="T5" s="43"/>
     </row>
-    <row r="6" spans="1:23" ht="19.5">
-      <c r="A6" s="50" t="s">
+    <row r="6" spans="1:24" ht="19.5">
+      <c r="A6" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="50"/>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="50"/>
-      <c r="H6" s="50"/>
-      <c r="I6" s="50"/>
-      <c r="J6" s="50"/>
-      <c r="K6" s="50"/>
-      <c r="L6" s="50"/>
-      <c r="M6" s="50"/>
-      <c r="N6" s="50"/>
-      <c r="O6" s="50"/>
-      <c r="P6" s="50"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="59"/>
+      <c r="G6" s="59"/>
+      <c r="H6" s="59"/>
+      <c r="I6" s="59"/>
+      <c r="J6" s="59"/>
+      <c r="K6" s="59"/>
+      <c r="L6" s="59"/>
+      <c r="M6" s="59"/>
+      <c r="N6" s="59"/>
+      <c r="O6" s="59"/>
+      <c r="P6" s="59"/>
       <c r="Q6" s="7"/>
       <c r="R6" s="44"/>
       <c r="S6" s="44"/>
       <c r="T6" s="44"/>
     </row>
-    <row r="7" spans="1:23" ht="19.5">
-      <c r="A7" s="50" t="s">
+    <row r="7" spans="1:24" ht="19.5">
+      <c r="A7" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="50"/>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="50"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="50"/>
-      <c r="J7" s="50"/>
-      <c r="K7" s="50"/>
-      <c r="L7" s="50"/>
-      <c r="M7" s="50"/>
-      <c r="N7" s="50"/>
-      <c r="O7" s="50"/>
-      <c r="P7" s="50"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="59"/>
+      <c r="G7" s="59"/>
+      <c r="H7" s="59"/>
+      <c r="I7" s="59"/>
+      <c r="J7" s="59"/>
+      <c r="K7" s="59"/>
+      <c r="L7" s="59"/>
+      <c r="M7" s="59"/>
+      <c r="N7" s="59"/>
+      <c r="O7" s="59"/>
+      <c r="P7" s="59"/>
       <c r="Q7" s="7"/>
       <c r="R7" s="44"/>
       <c r="S7" s="44"/>
       <c r="T7" s="44"/>
     </row>
-    <row r="8" spans="1:23" ht="13.5" thickBot="1">
-      <c r="A8" s="65" t="s">
+    <row r="8" spans="1:24" ht="13.5" thickBot="1">
+      <c r="A8" s="74" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="65"/>
-      <c r="C8" s="65"/>
-      <c r="D8" s="65"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="65"/>
-      <c r="G8" s="65"/>
-      <c r="H8" s="65"/>
-      <c r="I8" s="65"/>
-      <c r="J8" s="65"/>
-      <c r="K8" s="65"/>
-      <c r="L8" s="65"/>
-      <c r="M8" s="65"/>
-      <c r="N8" s="65"/>
-      <c r="O8" s="65"/>
-      <c r="P8" s="65"/>
+      <c r="B8" s="74"/>
+      <c r="C8" s="74"/>
+      <c r="D8" s="74"/>
+      <c r="E8" s="74"/>
+      <c r="F8" s="74"/>
+      <c r="G8" s="74"/>
+      <c r="H8" s="74"/>
+      <c r="I8" s="74"/>
+      <c r="J8" s="74"/>
+      <c r="K8" s="74"/>
+      <c r="L8" s="74"/>
+      <c r="M8" s="74"/>
+      <c r="N8" s="74"/>
+      <c r="O8" s="74"/>
+      <c r="P8" s="74"/>
       <c r="Q8" s="8"/>
       <c r="R8" s="45"/>
       <c r="S8" s="45"/>
       <c r="T8" s="45"/>
     </row>
-    <row r="9" spans="1:23" s="1" customFormat="1" ht="36.75" customHeight="1">
-      <c r="A9" s="61" t="s">
+    <row r="9" spans="1:24" s="1" customFormat="1" ht="36.75" customHeight="1">
+      <c r="A9" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="59" t="s">
+      <c r="B9" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="59" t="s">
+      <c r="C9" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="59" t="s">
+      <c r="D9" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="59" t="s">
+      <c r="E9" s="68" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="59" t="s">
+      <c r="F9" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="66" t="s">
+      <c r="G9" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="67"/>
-      <c r="I9" s="59"/>
-      <c r="J9" s="68" t="s">
+      <c r="H9" s="76"/>
+      <c r="I9" s="68"/>
+      <c r="J9" s="77" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="69"/>
-      <c r="L9" s="70"/>
-      <c r="M9" s="68" t="s">
+      <c r="K9" s="78"/>
+      <c r="L9" s="79"/>
+      <c r="M9" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="N9" s="69"/>
-      <c r="O9" s="70"/>
-      <c r="P9" s="71" t="s">
+      <c r="N9" s="78"/>
+      <c r="O9" s="79"/>
+      <c r="P9" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="Q9" s="54" t="s">
+      <c r="Q9" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="R9" s="55"/>
-      <c r="S9" s="55"/>
-      <c r="T9" s="56"/>
-      <c r="U9" s="63" t="s">
+      <c r="R9" s="64"/>
+      <c r="S9" s="64"/>
+      <c r="T9" s="65"/>
+      <c r="U9" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="V9" s="51" t="s">
+      <c r="V9" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="W9" s="53" t="s">
+      <c r="W9" s="62" t="s">
         <v>16</v>
       </c>
+      <c r="X9" s="54" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="10" spans="1:23" s="1" customFormat="1" ht="36.75" customHeight="1">
-      <c r="A10" s="62"/>
-      <c r="B10" s="60"/>
-      <c r="C10" s="60"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="60"/>
-      <c r="F10" s="60"/>
+    <row r="10" spans="1:24" s="1" customFormat="1" ht="36.75" customHeight="1">
+      <c r="A10" s="71"/>
+      <c r="B10" s="69"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="69"/>
       <c r="G10" s="2" t="s">
         <v>17</v>
       </c>
@@ -1356,7 +1369,7 @@
       <c r="O10" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="P10" s="64"/>
+      <c r="P10" s="73"/>
       <c r="Q10" s="12" t="s">
         <v>22</v>
       </c>
@@ -1369,11 +1382,12 @@
       <c r="T10" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="U10" s="64"/>
-      <c r="V10" s="52"/>
-      <c r="W10" s="53"/>
+      <c r="U10" s="73"/>
+      <c r="V10" s="61"/>
+      <c r="W10" s="62"/>
+      <c r="X10" s="54"/>
     </row>
-    <row r="11" spans="1:23" s="3" customFormat="1" ht="16.5" customHeight="1">
+    <row r="11" spans="1:24" s="3" customFormat="1" ht="16.5" customHeight="1">
       <c r="A11" s="21" t="s">
         <v>26</v>
       </c>
@@ -1401,40 +1415,40 @@
       <c r="I11" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="J11" s="72" t="s">
+      <c r="J11" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="K11" s="72" t="s">
+      <c r="K11" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="L11" s="72" t="s">
+      <c r="L11" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="M11" s="72" t="s">
+      <c r="M11" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="N11" s="72" t="s">
+      <c r="N11" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="O11" s="72" t="s">
+      <c r="O11" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="P11" s="73" t="s">
+      <c r="P11" s="47" t="s">
         <v>48</v>
       </c>
       <c r="Q11" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="R11" s="77" t="s">
+      <c r="R11" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="S11" s="77" t="s">
+      <c r="S11" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="T11" s="72" t="s">
+      <c r="T11" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="U11" s="73" t="s">
+      <c r="U11" s="47" t="s">
         <v>50</v>
       </c>
       <c r="V11" s="26" t="s">
@@ -1443,8 +1457,11 @@
       <c r="W11" s="27" t="s">
         <v>43</v>
       </c>
+      <c r="X11" s="14" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="12" spans="1:23" s="3" customFormat="1" ht="15.75" customHeight="1">
+    <row r="12" spans="1:24" s="3" customFormat="1" ht="15.75" customHeight="1">
       <c r="A12" s="16"/>
       <c r="B12" s="17"/>
       <c r="C12" s="18"/>
@@ -1454,94 +1471,96 @@
       <c r="G12" s="30"/>
       <c r="H12" s="18"/>
       <c r="I12" s="20"/>
-      <c r="J12" s="74"/>
-      <c r="K12" s="74"/>
-      <c r="L12" s="74"/>
-      <c r="M12" s="74"/>
-      <c r="N12" s="74"/>
-      <c r="O12" s="74"/>
-      <c r="P12" s="75"/>
+      <c r="J12" s="48"/>
+      <c r="K12" s="48"/>
+      <c r="L12" s="48"/>
+      <c r="M12" s="48"/>
+      <c r="N12" s="48"/>
+      <c r="O12" s="48"/>
+      <c r="P12" s="49"/>
       <c r="Q12" s="31"/>
-      <c r="R12" s="78"/>
-      <c r="S12" s="78"/>
-      <c r="T12" s="79"/>
-      <c r="U12" s="75"/>
+      <c r="R12" s="52"/>
+      <c r="S12" s="52"/>
+      <c r="T12" s="53"/>
+      <c r="U12" s="49"/>
       <c r="V12" s="15"/>
       <c r="W12" s="14"/>
+      <c r="X12" s="14"/>
     </row>
-    <row r="13" spans="1:23" s="1" customFormat="1" ht="36" customHeight="1" thickBot="1">
-      <c r="A13" s="57" t="s">
+    <row r="13" spans="1:24" s="1" customFormat="1" ht="36" customHeight="1" thickBot="1">
+      <c r="A13" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="58"/>
-      <c r="C13" s="58"/>
-      <c r="D13" s="58"/>
-      <c r="E13" s="58"/>
-      <c r="F13" s="58"/>
-      <c r="G13" s="58"/>
-      <c r="H13" s="58"/>
-      <c r="I13" s="58"/>
-      <c r="J13" s="76">
+      <c r="B13" s="67"/>
+      <c r="C13" s="67"/>
+      <c r="D13" s="67"/>
+      <c r="E13" s="67"/>
+      <c r="F13" s="67"/>
+      <c r="G13" s="67"/>
+      <c r="H13" s="67"/>
+      <c r="I13" s="67"/>
+      <c r="J13" s="50">
         <f t="shared" ref="J13:N13" si="0">SUM(J11:J12)</f>
         <v>0</v>
       </c>
-      <c r="K13" s="76">
+      <c r="K13" s="50">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L13" s="76">
+      <c r="L13" s="50">
         <f>SUM(L11:L12)</f>
         <v>0</v>
       </c>
-      <c r="M13" s="76">
+      <c r="M13" s="50">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N13" s="76">
+      <c r="N13" s="50">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O13" s="76">
+      <c r="O13" s="50">
         <f>SUM(O11:O12)</f>
         <v>0</v>
       </c>
-      <c r="P13" s="76">
+      <c r="P13" s="50">
         <f>SUM(P11:P12)</f>
         <v>0</v>
       </c>
       <c r="Q13" s="32"/>
-      <c r="R13" s="76">
+      <c r="R13" s="50">
         <f>SUM(R11:R12)</f>
         <v>0</v>
       </c>
-      <c r="S13" s="76">
+      <c r="S13" s="50">
         <f>SUM(S11:S12)</f>
         <v>0</v>
       </c>
-      <c r="T13" s="76">
+      <c r="T13" s="50">
         <f>SUM(T11:T12)</f>
         <v>0</v>
       </c>
-      <c r="U13" s="76">
+      <c r="U13" s="50">
         <f>SUM(U11:U12)</f>
         <v>0</v>
       </c>
       <c r="V13" s="13"/>
       <c r="W13" s="13"/>
+      <c r="X13" s="13"/>
     </row>
-    <row r="14" spans="1:23" ht="15.75">
+    <row r="14" spans="1:24" ht="15.75">
       <c r="N14" s="38"/>
       <c r="O14" s="38"/>
       <c r="P14" s="38"/>
       <c r="Q14" s="9"/>
     </row>
-    <row r="15" spans="1:23" ht="15.75">
+    <row r="15" spans="1:24" ht="15.75">
       <c r="N15" s="39"/>
       <c r="O15" s="39"/>
       <c r="P15" s="39"/>
       <c r="Q15" s="10"/>
     </row>
-    <row r="16" spans="1:23" ht="15.75">
+    <row r="16" spans="1:24" ht="15.75">
       <c r="N16" s="39"/>
       <c r="O16" s="39"/>
       <c r="P16" s="39"/>
@@ -1567,28 +1586,29 @@
     </row>
   </sheetData>
   <autoFilter ref="A9:W10"/>
-  <mergeCells count="21">
-    <mergeCell ref="A8:P8"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="M9:O9"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="V9:V10"/>
-    <mergeCell ref="W9:W10"/>
-    <mergeCell ref="Q9:T9"/>
+  <mergeCells count="22">
     <mergeCell ref="A13:I13"/>
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="E9:E10"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="B9:B10"/>
-    <mergeCell ref="U9:U10"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="X9:X10"/>
     <mergeCell ref="M2:P2"/>
     <mergeCell ref="A4:P4"/>
     <mergeCell ref="A5:P5"/>
     <mergeCell ref="A6:P6"/>
     <mergeCell ref="A7:P7"/>
+    <mergeCell ref="V9:V10"/>
+    <mergeCell ref="W9:W10"/>
+    <mergeCell ref="Q9:T9"/>
+    <mergeCell ref="U9:U10"/>
+    <mergeCell ref="A8:P8"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="P9:P10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1596,6 +1616,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002A5CA081AA03014D8863EFE0B1B9EF3A" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="edb9dd2956c3890b35d87d37ac778bb0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="41733dd2-07dd-4b83-9c00-dc1590a38c6d" xmlns:ns3="26469b81-5639-404a-a4db-d68c46bc65bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9c7b98c7a72137f7ed2cb8e1ee5f1d1b" ns2:_="" ns3:_="">
     <xsd:import namespace="41733dd2-07dd-4b83-9c00-dc1590a38c6d"/>
@@ -1798,16 +1827,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FE10460-D6AA-4897-8EBD-6EA94D1AC40D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{970E0757-8A16-4279-93C1-8DDDD52CCC3E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1824,12 +1852,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FE10460-D6AA-4897-8EBD-6EA94D1AC40D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
format righ ttemplate combine shipment
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/CombingBillingByJobUSD.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/CombingBillingByJobUSD.xlsx
@@ -572,7 +572,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -613,17 +613,11 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -635,9 +629,6 @@
     <xf numFmtId="1" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="37" fontId="9" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="37" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -689,6 +680,30 @@
     </xf>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -725,24 +740,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="39" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -751,12 +748,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="39" fontId="8" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -769,6 +760,12 @@
     </xf>
     <xf numFmtId="39" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="16">
@@ -1116,8 +1113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="X18" sqref="X18"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1130,218 +1127,218 @@
     <col min="6" max="6" width="29" customWidth="1"/>
     <col min="7" max="8" width="14" customWidth="1"/>
     <col min="9" max="9" width="16.5703125" customWidth="1"/>
-    <col min="10" max="16" width="20" style="34" customWidth="1"/>
+    <col min="10" max="16" width="20" style="31" customWidth="1"/>
     <col min="17" max="17" width="35.7109375" customWidth="1"/>
-    <col min="18" max="18" width="12.42578125" style="34" customWidth="1"/>
-    <col min="19" max="19" width="13" style="34" customWidth="1"/>
-    <col min="20" max="20" width="20" style="34" customWidth="1"/>
-    <col min="21" max="21" width="22" style="34" customWidth="1"/>
+    <col min="18" max="18" width="12.42578125" style="31" customWidth="1"/>
+    <col min="19" max="19" width="13" style="31" customWidth="1"/>
+    <col min="20" max="20" width="20" style="31" customWidth="1"/>
+    <col min="21" max="21" width="22" style="31" customWidth="1"/>
     <col min="22" max="22" width="15.85546875" customWidth="1"/>
     <col min="23" max="23" width="14.42578125" customWidth="1"/>
     <col min="24" max="24" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="20.25">
-      <c r="M1" s="35" t="s">
+      <c r="M1" s="32" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:24" ht="50.1" customHeight="1">
-      <c r="L2" s="36"/>
-      <c r="M2" s="55" t="s">
+      <c r="L2" s="33"/>
+      <c r="M2" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="N2" s="55"/>
-      <c r="O2" s="55"/>
-      <c r="P2" s="55"/>
+      <c r="N2" s="60"/>
+      <c r="O2" s="60"/>
+      <c r="P2" s="60"/>
       <c r="Q2" s="4"/>
-      <c r="R2" s="41"/>
-      <c r="S2" s="41"/>
-      <c r="T2" s="41"/>
+      <c r="R2" s="38"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="38"/>
     </row>
     <row r="4" spans="1:24" ht="20.25">
-      <c r="A4" s="56" t="s">
+      <c r="A4" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="56"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="56"/>
-      <c r="H4" s="56"/>
-      <c r="I4" s="56"/>
-      <c r="J4" s="56"/>
-      <c r="K4" s="56"/>
-      <c r="L4" s="56"/>
-      <c r="M4" s="56"/>
-      <c r="N4" s="56"/>
-      <c r="O4" s="56"/>
-      <c r="P4" s="56"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="61"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="61"/>
+      <c r="L4" s="61"/>
+      <c r="M4" s="61"/>
+      <c r="N4" s="61"/>
+      <c r="O4" s="61"/>
+      <c r="P4" s="61"/>
       <c r="Q4" s="5"/>
-      <c r="R4" s="42"/>
-      <c r="S4" s="42"/>
-      <c r="T4" s="42"/>
+      <c r="R4" s="39"/>
+      <c r="S4" s="39"/>
+      <c r="T4" s="39"/>
     </row>
     <row r="5" spans="1:24" ht="18.75">
-      <c r="A5" s="57" t="s">
+      <c r="A5" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="58"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="58"/>
-      <c r="E5" s="58"/>
-      <c r="F5" s="58"/>
-      <c r="G5" s="58"/>
-      <c r="H5" s="58"/>
-      <c r="I5" s="58"/>
-      <c r="J5" s="58"/>
-      <c r="K5" s="58"/>
-      <c r="L5" s="58"/>
-      <c r="M5" s="58"/>
-      <c r="N5" s="58"/>
-      <c r="O5" s="58"/>
-      <c r="P5" s="58"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="63"/>
+      <c r="I5" s="63"/>
+      <c r="J5" s="63"/>
+      <c r="K5" s="63"/>
+      <c r="L5" s="63"/>
+      <c r="M5" s="63"/>
+      <c r="N5" s="63"/>
+      <c r="O5" s="63"/>
+      <c r="P5" s="63"/>
       <c r="Q5" s="6"/>
-      <c r="R5" s="43"/>
-      <c r="S5" s="43"/>
-      <c r="T5" s="43"/>
+      <c r="R5" s="40"/>
+      <c r="S5" s="40"/>
+      <c r="T5" s="40"/>
     </row>
     <row r="6" spans="1:24" ht="19.5">
-      <c r="A6" s="59" t="s">
+      <c r="A6" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="59"/>
-      <c r="C6" s="59"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="59"/>
-      <c r="H6" s="59"/>
-      <c r="I6" s="59"/>
-      <c r="J6" s="59"/>
-      <c r="K6" s="59"/>
-      <c r="L6" s="59"/>
-      <c r="M6" s="59"/>
-      <c r="N6" s="59"/>
-      <c r="O6" s="59"/>
-      <c r="P6" s="59"/>
+      <c r="B6" s="64"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="64"/>
+      <c r="H6" s="64"/>
+      <c r="I6" s="64"/>
+      <c r="J6" s="64"/>
+      <c r="K6" s="64"/>
+      <c r="L6" s="64"/>
+      <c r="M6" s="64"/>
+      <c r="N6" s="64"/>
+      <c r="O6" s="64"/>
+      <c r="P6" s="64"/>
       <c r="Q6" s="7"/>
-      <c r="R6" s="44"/>
-      <c r="S6" s="44"/>
-      <c r="T6" s="44"/>
+      <c r="R6" s="41"/>
+      <c r="S6" s="41"/>
+      <c r="T6" s="41"/>
     </row>
     <row r="7" spans="1:24" ht="19.5">
-      <c r="A7" s="59" t="s">
+      <c r="A7" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="59"/>
-      <c r="C7" s="59"/>
-      <c r="D7" s="59"/>
-      <c r="E7" s="59"/>
-      <c r="F7" s="59"/>
-      <c r="G7" s="59"/>
-      <c r="H7" s="59"/>
-      <c r="I7" s="59"/>
-      <c r="J7" s="59"/>
-      <c r="K7" s="59"/>
-      <c r="L7" s="59"/>
-      <c r="M7" s="59"/>
-      <c r="N7" s="59"/>
-      <c r="O7" s="59"/>
-      <c r="P7" s="59"/>
+      <c r="B7" s="64"/>
+      <c r="C7" s="64"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="64"/>
+      <c r="H7" s="64"/>
+      <c r="I7" s="64"/>
+      <c r="J7" s="64"/>
+      <c r="K7" s="64"/>
+      <c r="L7" s="64"/>
+      <c r="M7" s="64"/>
+      <c r="N7" s="64"/>
+      <c r="O7" s="64"/>
+      <c r="P7" s="64"/>
       <c r="Q7" s="7"/>
-      <c r="R7" s="44"/>
-      <c r="S7" s="44"/>
-      <c r="T7" s="44"/>
+      <c r="R7" s="41"/>
+      <c r="S7" s="41"/>
+      <c r="T7" s="41"/>
     </row>
     <row r="8" spans="1:24" ht="13.5" thickBot="1">
-      <c r="A8" s="74" t="s">
+      <c r="A8" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="74"/>
-      <c r="C8" s="74"/>
-      <c r="D8" s="74"/>
-      <c r="E8" s="74"/>
-      <c r="F8" s="74"/>
-      <c r="G8" s="74"/>
-      <c r="H8" s="74"/>
-      <c r="I8" s="74"/>
-      <c r="J8" s="74"/>
-      <c r="K8" s="74"/>
-      <c r="L8" s="74"/>
-      <c r="M8" s="74"/>
-      <c r="N8" s="74"/>
-      <c r="O8" s="74"/>
-      <c r="P8" s="74"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="73"/>
+      <c r="G8" s="73"/>
+      <c r="H8" s="73"/>
+      <c r="I8" s="73"/>
+      <c r="J8" s="73"/>
+      <c r="K8" s="73"/>
+      <c r="L8" s="73"/>
+      <c r="M8" s="73"/>
+      <c r="N8" s="73"/>
+      <c r="O8" s="73"/>
+      <c r="P8" s="73"/>
       <c r="Q8" s="8"/>
-      <c r="R8" s="45"/>
-      <c r="S8" s="45"/>
-      <c r="T8" s="45"/>
+      <c r="R8" s="42"/>
+      <c r="S8" s="42"/>
+      <c r="T8" s="42"/>
     </row>
     <row r="9" spans="1:24" s="1" customFormat="1" ht="36.75" customHeight="1">
-      <c r="A9" s="70" t="s">
+      <c r="A9" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="68" t="s">
+      <c r="B9" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="68" t="s">
+      <c r="C9" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="68" t="s">
+      <c r="D9" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="68" t="s">
+      <c r="E9" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="68" t="s">
+      <c r="F9" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="75" t="s">
+      <c r="G9" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="76"/>
-      <c r="I9" s="68"/>
-      <c r="J9" s="77" t="s">
+      <c r="H9" s="58"/>
+      <c r="I9" s="53"/>
+      <c r="J9" s="74" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="78"/>
-      <c r="L9" s="79"/>
-      <c r="M9" s="77" t="s">
+      <c r="K9" s="75"/>
+      <c r="L9" s="76"/>
+      <c r="M9" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="N9" s="78"/>
-      <c r="O9" s="79"/>
-      <c r="P9" s="80" t="s">
+      <c r="N9" s="75"/>
+      <c r="O9" s="76"/>
+      <c r="P9" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="Q9" s="63" t="s">
+      <c r="Q9" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="R9" s="64"/>
-      <c r="S9" s="64"/>
-      <c r="T9" s="65"/>
-      <c r="U9" s="72" t="s">
+      <c r="R9" s="69"/>
+      <c r="S9" s="69"/>
+      <c r="T9" s="70"/>
+      <c r="U9" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="V9" s="60" t="s">
+      <c r="V9" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="W9" s="62" t="s">
+      <c r="W9" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="X9" s="54" t="s">
+      <c r="X9" s="59" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:24" s="1" customFormat="1" ht="36.75" customHeight="1">
-      <c r="A10" s="71"/>
-      <c r="B10" s="69"/>
-      <c r="C10" s="69"/>
-      <c r="D10" s="69"/>
-      <c r="E10" s="69"/>
-      <c r="F10" s="69"/>
+      <c r="A10" s="56"/>
+      <c r="B10" s="54"/>
+      <c r="C10" s="54"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="54"/>
       <c r="G10" s="2" t="s">
         <v>17</v>
       </c>
@@ -1351,110 +1348,110 @@
       <c r="I10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="37" t="s">
+      <c r="J10" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="K10" s="37" t="s">
+      <c r="K10" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="L10" s="37" t="s">
+      <c r="L10" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="M10" s="37" t="s">
+      <c r="M10" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="N10" s="37" t="s">
+      <c r="N10" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="O10" s="37" t="s">
+      <c r="O10" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="P10" s="73"/>
+      <c r="P10" s="72"/>
       <c r="Q10" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="R10" s="37" t="s">
+      <c r="R10" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="S10" s="37" t="s">
+      <c r="S10" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="T10" s="37" t="s">
+      <c r="T10" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="U10" s="73"/>
-      <c r="V10" s="61"/>
-      <c r="W10" s="62"/>
-      <c r="X10" s="54"/>
+      <c r="U10" s="72"/>
+      <c r="V10" s="66"/>
+      <c r="W10" s="67"/>
+      <c r="X10" s="59"/>
     </row>
     <row r="11" spans="1:24" s="3" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="28" t="s">
+      <c r="D11" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="25" t="s">
+      <c r="E11" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="23" t="s">
+      <c r="F11" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="G11" s="28" t="s">
+      <c r="G11" s="78" t="s">
         <v>42</v>
       </c>
-      <c r="H11" s="23" t="s">
+      <c r="H11" s="78" t="s">
         <v>32</v>
       </c>
-      <c r="I11" s="24" t="s">
+      <c r="I11" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="J11" s="46" t="s">
+      <c r="J11" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="K11" s="46" t="s">
+      <c r="K11" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="L11" s="46" t="s">
+      <c r="L11" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="M11" s="46" t="s">
+      <c r="M11" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="N11" s="46" t="s">
+      <c r="N11" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="O11" s="46" t="s">
+      <c r="O11" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="P11" s="47" t="s">
+      <c r="P11" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="Q11" s="33" t="s">
+      <c r="Q11" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="R11" s="51" t="s">
+      <c r="R11" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="S11" s="51" t="s">
+      <c r="S11" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="T11" s="46" t="s">
+      <c r="T11" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="U11" s="47" t="s">
+      <c r="U11" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="V11" s="26" t="s">
+      <c r="V11" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="W11" s="27" t="s">
+      <c r="W11" s="25" t="s">
         <v>43</v>
       </c>
       <c r="X11" s="14" t="s">
@@ -1465,82 +1462,82 @@
       <c r="A12" s="16"/>
       <c r="B12" s="17"/>
       <c r="C12" s="18"/>
-      <c r="D12" s="29"/>
+      <c r="D12" s="27"/>
       <c r="E12" s="19"/>
       <c r="F12" s="18"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="48"/>
-      <c r="K12" s="48"/>
-      <c r="L12" s="48"/>
-      <c r="M12" s="48"/>
-      <c r="N12" s="48"/>
-      <c r="O12" s="48"/>
-      <c r="P12" s="49"/>
-      <c r="Q12" s="31"/>
-      <c r="R12" s="52"/>
-      <c r="S12" s="52"/>
-      <c r="T12" s="53"/>
-      <c r="U12" s="49"/>
+      <c r="G12" s="79"/>
+      <c r="H12" s="79"/>
+      <c r="I12" s="79"/>
+      <c r="J12" s="45"/>
+      <c r="K12" s="45"/>
+      <c r="L12" s="45"/>
+      <c r="M12" s="45"/>
+      <c r="N12" s="45"/>
+      <c r="O12" s="45"/>
+      <c r="P12" s="46"/>
+      <c r="Q12" s="28"/>
+      <c r="R12" s="49"/>
+      <c r="S12" s="49"/>
+      <c r="T12" s="50"/>
+      <c r="U12" s="46"/>
       <c r="V12" s="15"/>
       <c r="W12" s="14"/>
       <c r="X12" s="14"/>
     </row>
     <row r="13" spans="1:24" s="1" customFormat="1" ht="36" customHeight="1" thickBot="1">
-      <c r="A13" s="66" t="s">
+      <c r="A13" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="67"/>
-      <c r="C13" s="67"/>
-      <c r="D13" s="67"/>
-      <c r="E13" s="67"/>
-      <c r="F13" s="67"/>
-      <c r="G13" s="67"/>
-      <c r="H13" s="67"/>
-      <c r="I13" s="67"/>
-      <c r="J13" s="50">
+      <c r="B13" s="52"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="52"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="47">
         <f t="shared" ref="J13:N13" si="0">SUM(J11:J12)</f>
         <v>0</v>
       </c>
-      <c r="K13" s="50">
+      <c r="K13" s="47">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L13" s="50">
+      <c r="L13" s="47">
         <f>SUM(L11:L12)</f>
         <v>0</v>
       </c>
-      <c r="M13" s="50">
+      <c r="M13" s="47">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N13" s="50">
+      <c r="N13" s="47">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O13" s="50">
+      <c r="O13" s="47">
         <f>SUM(O11:O12)</f>
         <v>0</v>
       </c>
-      <c r="P13" s="50">
+      <c r="P13" s="47">
         <f>SUM(P11:P12)</f>
         <v>0</v>
       </c>
-      <c r="Q13" s="32"/>
-      <c r="R13" s="50">
+      <c r="Q13" s="29"/>
+      <c r="R13" s="47">
         <f>SUM(R11:R12)</f>
         <v>0</v>
       </c>
-      <c r="S13" s="50">
+      <c r="S13" s="47">
         <f>SUM(S11:S12)</f>
         <v>0</v>
       </c>
-      <c r="T13" s="50">
+      <c r="T13" s="47">
         <f>SUM(T11:T12)</f>
         <v>0</v>
       </c>
-      <c r="U13" s="50">
+      <c r="U13" s="47">
         <f>SUM(U11:U12)</f>
         <v>0</v>
       </c>
@@ -1549,52 +1546,44 @@
       <c r="X13" s="13"/>
     </row>
     <row r="14" spans="1:24" ht="15.75">
-      <c r="N14" s="38"/>
-      <c r="O14" s="38"/>
-      <c r="P14" s="38"/>
+      <c r="N14" s="35"/>
+      <c r="O14" s="35"/>
+      <c r="P14" s="35"/>
       <c r="Q14" s="9"/>
     </row>
     <row r="15" spans="1:24" ht="15.75">
-      <c r="N15" s="39"/>
-      <c r="O15" s="39"/>
-      <c r="P15" s="39"/>
+      <c r="N15" s="36"/>
+      <c r="O15" s="36"/>
+      <c r="P15" s="36"/>
       <c r="Q15" s="10"/>
     </row>
     <row r="16" spans="1:24" ht="15.75">
-      <c r="N16" s="39"/>
-      <c r="O16" s="39"/>
-      <c r="P16" s="39"/>
+      <c r="N16" s="36"/>
+      <c r="O16" s="36"/>
+      <c r="P16" s="36"/>
       <c r="Q16" s="10"/>
     </row>
     <row r="17" spans="14:17" ht="15.75">
-      <c r="N17" s="39"/>
-      <c r="O17" s="39"/>
-      <c r="P17" s="39"/>
+      <c r="N17" s="36"/>
+      <c r="O17" s="36"/>
+      <c r="P17" s="36"/>
       <c r="Q17" s="10"/>
     </row>
     <row r="18" spans="14:17" ht="15.75">
-      <c r="N18" s="40"/>
-      <c r="O18" s="40"/>
-      <c r="P18" s="40"/>
+      <c r="N18" s="37"/>
+      <c r="O18" s="37"/>
+      <c r="P18" s="37"/>
       <c r="Q18" s="11"/>
     </row>
     <row r="19" spans="14:17" ht="15.75">
-      <c r="N19" s="40"/>
-      <c r="O19" s="40"/>
-      <c r="P19" s="40"/>
+      <c r="N19" s="37"/>
+      <c r="O19" s="37"/>
+      <c r="P19" s="37"/>
       <c r="Q19" s="11"/>
     </row>
   </sheetData>
   <autoFilter ref="A9:W10"/>
   <mergeCells count="22">
-    <mergeCell ref="A13:I13"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
     <mergeCell ref="X9:X10"/>
     <mergeCell ref="M2:P2"/>
     <mergeCell ref="A4:P4"/>
@@ -1609,6 +1598,14 @@
     <mergeCell ref="J9:L9"/>
     <mergeCell ref="M9:O9"/>
     <mergeCell ref="P9:P10"/>
+    <mergeCell ref="A13:I13"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1616,15 +1613,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002A5CA081AA03014D8863EFE0B1B9EF3A" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="edb9dd2956c3890b35d87d37ac778bb0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="41733dd2-07dd-4b83-9c00-dc1590a38c6d" xmlns:ns3="26469b81-5639-404a-a4db-d68c46bc65bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9c7b98c7a72137f7ed2cb8e1ee5f1d1b" ns2:_="" ns3:_="">
     <xsd:import namespace="41733dd2-07dd-4b83-9c00-dc1590a38c6d"/>
@@ -1827,15 +1815,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FE10460-D6AA-4897-8EBD-6EA94D1AC40D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{970E0757-8A16-4279-93C1-8DDDD52CCC3E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1852,4 +1841,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FE10460-D6AA-4897-8EBD-6EA94D1AC40D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>